<commit_message>
feat: add custom scenario for transportation
</commit_message>
<xml_diff>
--- a/references/background_data/a4_emissions.xlsx
+++ b/references/background_data/a4_emissions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_scenario_explorer\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268C8533-479E-4325-B00D-30236A9B2912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1075F8-F927-4B50-909B-2C11CAB0DBE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Product system name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Reference</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>1 tkm</t>
@@ -930,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,30 +938,30 @@
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -972,13 +969,10 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>3.5199999999999999E-4</v>
@@ -989,6 +983,12 @@
       <c r="D2">
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2" s="1">
         <v>2.0000000000000001E-10</v>
       </c>
@@ -996,15 +996,15 @@
         <v>9.6100000000000005E-3</v>
       </c>
       <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>3.7399999999999998E-4</v>
@@ -1015,6 +1015,12 @@
       <c r="D3">
         <v>2.1999999999999999E-2</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3" s="1">
         <v>1.35E-10</v>
       </c>
@@ -1022,15 +1028,15 @@
         <v>1.29E-2</v>
       </c>
       <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>4.8000000000000001E-4</v>
@@ -1041,6 +1047,12 @@
       <c r="D4">
         <v>9.4E-2</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="G4" s="1">
         <v>5.68E-10</v>
       </c>
@@ -1048,15 +1060,15 @@
         <v>1.54E-2</v>
       </c>
       <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>3.6499999999999998E-4</v>
@@ -1067,6 +1079,12 @@
       <c r="D5">
         <v>1.9E-2</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5" s="1">
         <v>1.11E-10</v>
       </c>
@@ -1074,16 +1092,16 @@
         <v>1.12E-2</v>
       </c>
       <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>